<commit_message>
Primer DRAFT con error
No pude mergear la base df con la de adulto equivalente, si alguien la puede hacer, lo otro ya estaría de la parte. OJO, respetar los nombres porque sino lo de abajo no va a funcionar

Co-Authored-By: Juan Diego Barnes <144281917+JuanDBarnes@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/TP2/tabla_adulto_equiv.xlsx
+++ b/TP2/tabla_adulto_equiv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pupih\Desktop\EPH_usu_1_Trim_2019_xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Escritorio\Maestría\Big Data\BigData\TP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E962F3C-29E4-4745-A82B-33515FD15C1A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59D7502-3917-431D-BEA8-7F34B8186645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="20370" yWindow="-5985" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla de adulo equivalente" sheetId="7" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Edad</t>
   </si>
@@ -106,83 +106,19 @@
   </si>
   <si>
     <t>más de 75 años</t>
-  </si>
-  <si>
-    <t>Ejemplos de determinación de las unidades consumidoras (adultos equivalentes)</t>
-  </si>
-  <si>
-    <t>Se presentan a continuación tres ejemplos de cómo se determina la cantidad de unidades consumidoras (adultos equivalentes) para diferentes hogares.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Fuente: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>INDEC.</t>
-    </r>
-  </si>
-  <si>
-    <t>Tabla de equivalencias de necesidades energéticas. Unidades de adulto equivalente, según sexo y edad</t>
-  </si>
-  <si>
-    <t>Hogar 1: de tres integrantes, compuesto por una mujer de 35 años, su hijo de 18 años y su madre de 61 años. En total, el hogar suma  2,46 adultos equivalentes.</t>
-  </si>
-  <si>
-    <t>Hogar 2: de cuatro integrantes, compuesto por un varón de 35 años, una mujer de 31 años, un hijo de 6 años y una hija de 8 años. En total, el hogar suma 3,09 adultos equivalentes</t>
-  </si>
-  <si>
-    <t>Hogar 3: de cinco integrantes, constituido por una pareja de un varón y una mujer, ambos de 30 años, y tres hijos de 5, 3 y 1 año. En total, el hogar suma 3,25 adultos equivalentes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="4"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -198,27 +134,8 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -273,54 +190,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -339,9 +238,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -379,9 +278,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -414,26 +313,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -466,26 +348,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -658,424 +523,341 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-    </row>
-    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B2" s="5">
         <v>0.35</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C2" s="5">
         <v>0.35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B3" s="5">
         <v>0.37</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C3" s="5">
         <v>0.37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B4" s="5">
         <v>0.46</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C4" s="5">
         <v>0.46</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B5" s="5">
         <v>0.51</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C5" s="5">
         <v>0.51</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B6" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C6" s="5">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0.64</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.66</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.68</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B11" s="6">
-        <v>0.6</v>
+        <v>0.69</v>
       </c>
       <c r="C11" s="6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="6">
-        <v>0.66</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="6">
-        <v>0.68</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="7">
         <v>0.69</v>
       </c>
-      <c r="C15" s="7">
-        <v>0.69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B12" s="5">
         <v>0.7</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C12" s="5">
         <v>0.79</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B13" s="5">
         <v>0.72</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C13" s="5">
         <v>0.82</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B14" s="5">
         <v>0.74</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C14" s="5">
         <v>0.85</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B15" s="5">
         <v>0.76</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C15" s="5">
         <v>0.9</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B16" s="5">
         <v>0.76</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C16" s="5">
         <v>0.96</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B17" s="5">
         <v>0.77</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C17" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B18" s="5">
         <v>0.77</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C18" s="5">
         <v>1.03</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B19" s="5">
         <v>0.77</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C19" s="5">
         <v>1.04</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B20" s="5">
         <v>0.76</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C20" s="5">
         <v>1.02</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B21" s="5">
         <v>0.77</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C21" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B22" s="5">
         <v>0.76</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C22" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B23" s="5">
         <v>0.67</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C23" s="5">
         <v>0.83</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B24" s="8">
         <v>0.63</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C24" s="8">
         <v>0.74</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-    </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
+    <row r="25" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="A31:D32"/>
-    <mergeCell ref="A33:D34"/>
-    <mergeCell ref="A35:D36"/>
-    <mergeCell ref="A37:D38"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>